<commit_message>
se aplica algoritmo de hilo para poder ejecutar varios codigos a la vez
</commit_message>
<xml_diff>
--- a/Control Stock Web 2024-07-04.xlsx
+++ b/Control Stock Web 2024-07-04.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,7 +446,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>10950134003</t>
+          <t>10930745010</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -456,17 +456,17 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>$ 62.993</t>
+          <t>$ 182.990</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>10950134004</t>
+          <t>10962389016</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -476,70 +476,10 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>$ 62.993</t>
+          <t>$ 165.990</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>10242985001</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Disponible</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>$ 17.990</t>
-        </is>
-      </c>
-      <c r="D4" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>10950134002</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Disponible</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>$ 62.993</t>
-        </is>
-      </c>
-      <c r="D5" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>10950134005</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Disponible</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>$ 62.993</t>
-        </is>
-      </c>
-      <c r="D6" t="n">
         <v>3</v>
       </c>
     </row>

</xml_diff>